<commit_message>
AdminModuleTest class get created
</commit_message>
<xml_diff>
--- a/excel/loginData.xlsx
+++ b/excel/loginData.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="AdminModuleTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -37,15 +37,9 @@
     <t>admin123</t>
   </si>
   <si>
-    <t>admin124</t>
-  </si>
-  <si>
     <t>testLoginWithValidCredentials</t>
   </si>
   <si>
-    <t>testLoginWithValidCredentials1</t>
-  </si>
-  <si>
     <t>testLoginWithInvalidCredentials</t>
   </si>
   <si>
@@ -53,6 +47,12 @@
   </si>
   <si>
     <t>madmin123</t>
+  </si>
+  <si>
+    <t>validateIfAdminPageOpenSuccessfully</t>
+  </si>
+  <si>
+    <t>searchSystemUsersBasedOnBelowNames</t>
   </si>
 </sst>
 </file>
@@ -372,8 +372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -396,7 +396,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -407,13 +407,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -424,37 +424,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.7265625" customWidth="1"/>
+    <col min="1" max="1" width="32.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>